<commit_message>
change vs2012 project to vs2013 project.
</commit_message>
<xml_diff>
--- a/doc/中间代码到目标代码映射关系.xlsx
+++ b/doc/中间代码到目标代码映射关系.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6360" yWindow="0" windowWidth="18900" windowHeight="8355"/>
+    <workbookView xWindow="7950" yWindow="0" windowWidth="18900" windowHeight="8355"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -66,10 +66,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>r      a</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>DL</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -385,10 +381,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>r        a</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>r        b</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -516,6 +508,14 @@
   </si>
   <si>
     <t>MOV</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>r      b</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>r        b</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -674,16 +674,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -968,8 +968,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="L40" sqref="L40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -981,7 +981,7 @@
   <sheetData>
     <row r="1" spans="1:23" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -1014,25 +1014,25 @@
         <v>9</v>
       </c>
       <c r="M1" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="N1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q1" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="O1" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>47</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>48</v>
       </c>
       <c r="T1" s="3"/>
       <c r="U1" s="3"/>
@@ -1044,55 +1044,55 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="G2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="I2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="J2" s="2" t="s">
-        <v>34</v>
-      </c>
       <c r="K2" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="M2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="T2" s="3"/>
       <c r="U2" s="3"/>
@@ -1104,55 +1104,55 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>16</v>
-      </c>
       <c r="E3" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="N3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="P3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="O3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="P3" s="2" t="s">
-        <v>16</v>
-      </c>
       <c r="Q3" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="S3" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="T3" s="3"/>
       <c r="U3" s="3"/>
@@ -1164,55 +1164,55 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>41</v>
-      </c>
       <c r="E4" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="J4" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="J4" s="2" t="s">
-        <v>37</v>
-      </c>
       <c r="K4" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="N4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="P4" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="O4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="P4" s="2" t="s">
-        <v>41</v>
-      </c>
       <c r="Q4" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="S4" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="T4" s="3"/>
       <c r="U4" s="3"/>
@@ -1224,58 +1224,58 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="D5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="F5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="G5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="I5" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="J5" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="J5" s="2" t="s">
-        <v>39</v>
-      </c>
       <c r="K5" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L5" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="M5" s="2" t="s">
         <v>3</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="P5" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="Q5" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="R5" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="S5" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="T5" s="3"/>
       <c r="U5" s="3"/>
@@ -1287,58 +1287,58 @@
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L6" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="M6" s="2" t="s">
         <v>4</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="O6" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="P6" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="Q6" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="R6" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="S6" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="T6" s="3"/>
       <c r="U6" s="3"/>
@@ -1350,58 +1350,58 @@
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L7" s="5" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="M7" s="2" t="s">
         <v>5</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="O7" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="P7" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="Q7" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="R7" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="S7" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="T7" s="3"/>
       <c r="U7" s="3"/>
@@ -1413,56 +1413,56 @@
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="D8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="I8" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L8" s="6"/>
       <c r="M8" s="2" t="s">
         <v>6</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="O8" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="P8" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="Q8" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="R8" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="S8" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="T8" s="3"/>
       <c r="U8" s="3"/>
@@ -1474,56 +1474,56 @@
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L9" s="6"/>
       <c r="M9" s="2" t="s">
         <v>7</v>
       </c>
       <c r="N9" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="O9" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="P9" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Q9" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="R9" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="S9" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="T9" s="3"/>
       <c r="U9" s="3"/>
@@ -1535,55 +1535,55 @@
         <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M10" s="2" t="s">
         <v>8</v>
       </c>
       <c r="N10" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="O10" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="P10" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="Q10" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="R10" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="S10" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="T10" s="3"/>
       <c r="U10" s="3"/>
@@ -1595,55 +1595,55 @@
         <v>9</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C11" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K11" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="I11" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="J11" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="K11" s="2" t="s">
-        <v>22</v>
       </c>
       <c r="M11" s="2" t="s">
         <v>9</v>
       </c>
       <c r="N11" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="O11" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P11" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q11" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="Q11" s="2" t="s">
-        <v>21</v>
-      </c>
       <c r="R11" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="S11" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="T11" s="3"/>
       <c r="U11" s="3"/>
@@ -1652,7 +1652,7 @@
     </row>
     <row r="13" spans="1:23" ht="27" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>0</v>
@@ -1690,34 +1690,34 @@
         <v>0</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.15">
@@ -1725,34 +1725,34 @@
         <v>1</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G15" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="I15" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="H15" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="I15" s="2" t="s">
-        <v>60</v>
-      </c>
       <c r="J15" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.15">
@@ -1760,34 +1760,34 @@
         <v>2</v>
       </c>
       <c r="B16" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C16" s="2" t="s">
-        <v>55</v>
-      </c>
       <c r="D16" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F16" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="E16" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>55</v>
-      </c>
       <c r="G16" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H16" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="I16" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="I16" s="2" t="s">
-        <v>60</v>
-      </c>
       <c r="J16" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.15">
@@ -1795,37 +1795,37 @@
         <v>3</v>
       </c>
       <c r="B17" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C17" s="2" t="s">
-        <v>55</v>
-      </c>
       <c r="D17" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E17" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F17" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="F17" s="2" t="s">
-        <v>55</v>
-      </c>
       <c r="G17" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.15">
@@ -1833,34 +1833,34 @@
         <v>4</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.15">
@@ -1868,34 +1868,34 @@
         <v>5</v>
       </c>
       <c r="B19" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F19" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C19" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>55</v>
-      </c>
       <c r="G19" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:23" x14ac:dyDescent="0.15">
@@ -1903,34 +1903,34 @@
         <v>6</v>
       </c>
       <c r="B20" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D20" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="E20" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F20" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D20" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="E20" s="2" t="s">
+      <c r="G20" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="F20" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>55</v>
-      </c>
       <c r="H20" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="21" spans="1:23" x14ac:dyDescent="0.15">
@@ -1938,34 +1938,34 @@
         <v>7</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:23" x14ac:dyDescent="0.15">
@@ -1973,34 +1973,34 @@
         <v>8</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:23" x14ac:dyDescent="0.15">
@@ -2008,39 +2008,39 @@
         <v>9</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="25" spans="1:23" ht="21.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>0</v>
@@ -2073,7 +2073,7 @@
         <v>9</v>
       </c>
       <c r="M25" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="N25" s="2" t="s">
         <v>0</v>
@@ -2111,67 +2111,67 @@
         <v>0</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K26" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M26" s="2" t="s">
         <v>0</v>
       </c>
       <c r="N26" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="O26" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="O26" s="2" t="s">
-        <v>72</v>
-      </c>
       <c r="P26" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="Q26" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="R26" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="S26" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="T26" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="U26" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="V26" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="W26" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="27" spans="1:23" x14ac:dyDescent="0.15">
@@ -2179,67 +2179,67 @@
         <v>1</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M27" s="2" t="s">
         <v>1</v>
       </c>
       <c r="N27" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="O27" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="P27" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="Q27" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="R27" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="S27" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="T27" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="U27" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="V27" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="W27" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="28" spans="1:23" x14ac:dyDescent="0.15">
@@ -2247,70 +2247,70 @@
         <v>2</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L28" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="M28" s="2" t="s">
         <v>2</v>
       </c>
       <c r="N28" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="O28" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="O28" s="2" t="s">
-        <v>72</v>
-      </c>
       <c r="P28" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="Q28" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="R28" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="S28" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="T28" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="U28" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="V28" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="W28" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="29" spans="1:23" x14ac:dyDescent="0.15">
@@ -2318,67 +2318,67 @@
         <v>3</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M29" s="2" t="s">
         <v>3</v>
       </c>
       <c r="N29" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="O29" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="O29" s="2" t="s">
-        <v>72</v>
-      </c>
       <c r="P29" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="Q29" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="R29" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="S29" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="T29" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="U29" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="V29" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="W29" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="30" spans="1:23" x14ac:dyDescent="0.15">
@@ -2386,70 +2386,70 @@
         <v>4</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K30" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L30" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="M30" s="2" t="s">
         <v>4</v>
       </c>
       <c r="N30" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="O30" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="O30" s="2" t="s">
-        <v>72</v>
-      </c>
       <c r="P30" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="Q30" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="R30" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="S30" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="T30" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="U30" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="V30" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="W30" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="31" spans="1:23" x14ac:dyDescent="0.15">
@@ -2457,70 +2457,70 @@
         <v>5</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K31" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L31" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="M31" s="2" t="s">
         <v>5</v>
       </c>
       <c r="N31" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="O31" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="O31" s="2" t="s">
-        <v>72</v>
-      </c>
       <c r="P31" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="Q31" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="R31" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="S31" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="T31" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="U31" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="V31" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="W31" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="32" spans="1:23" x14ac:dyDescent="0.15">
@@ -2528,70 +2528,70 @@
         <v>6</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K32" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L32" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="M32" s="2" t="s">
         <v>6</v>
       </c>
       <c r="N32" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="O32" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="O32" s="2" t="s">
-        <v>72</v>
-      </c>
       <c r="P32" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="Q32" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="R32" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="S32" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="T32" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="U32" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="V32" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="W32" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="33" spans="1:23" x14ac:dyDescent="0.15">
@@ -2599,67 +2599,67 @@
         <v>7</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J33" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K33" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M33" s="2" t="s">
         <v>7</v>
       </c>
       <c r="N33" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="O33" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="P33" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="Q33" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="R33" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="S33" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="T33" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="U33" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="V33" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="W33" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="34" spans="1:23" x14ac:dyDescent="0.15">
@@ -2667,67 +2667,67 @@
         <v>8</v>
       </c>
       <c r="B34" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="I34" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="J34" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="D34" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="F34" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="G34" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="H34" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="I34" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="J34" s="2" t="s">
-        <v>70</v>
-      </c>
       <c r="K34" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="M34" s="2" t="s">
         <v>8</v>
       </c>
       <c r="N34" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="O34" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="P34" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q34" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="R34" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="S34" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="T34" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="U34" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="O34" s="2" t="s">
+      <c r="V34" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="P34" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="Q34" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="R34" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="S34" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="T34" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="U34" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="V34" s="2" t="s">
-        <v>70</v>
-      </c>
       <c r="W34" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="35" spans="1:23" x14ac:dyDescent="0.15">
@@ -2735,77 +2735,77 @@
         <v>9</v>
       </c>
       <c r="B35" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H35" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I35" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C35" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F35" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G35" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="H35" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I35" s="2" t="s">
-        <v>21</v>
-      </c>
       <c r="J35" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K35" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="M35" s="2" t="s">
         <v>9</v>
       </c>
       <c r="N35" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="O35" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="P35" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q35" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="R35" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="S35" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="T35" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="U35" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="V35" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="W35" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="36" spans="1:23" ht="27" x14ac:dyDescent="0.15">
       <c r="L36" s="8" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="37" spans="1:23" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="1" t="s">
-        <v>10</v>
+        <v>120</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>0</v>
@@ -2838,7 +2838,7 @@
         <v>9</v>
       </c>
       <c r="M37" s="1" t="s">
-        <v>89</v>
+        <v>121</v>
       </c>
       <c r="N37" s="2" t="s">
         <v>0</v>
@@ -2876,67 +2876,67 @@
         <v>0</v>
       </c>
       <c r="B38" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C38" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="D38" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="F38" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D38" s="2" t="s">
+      <c r="G38" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="E38" s="2" t="s">
+      <c r="H38" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="F38" s="2" t="s">
+      <c r="I38" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="G38" s="2" t="s">
+      <c r="J38" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="H38" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="I38" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="J38" s="2" t="s">
-        <v>79</v>
-      </c>
       <c r="K38" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M38" s="2" t="s">
         <v>0</v>
       </c>
       <c r="N38" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="O38" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="P38" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="O38" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="P38" s="2" t="s">
+      <c r="Q38" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="R38" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="Q38" s="2" t="s">
+      <c r="S38" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="R38" s="2" t="s">
+      <c r="T38" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="U38" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="S38" s="2" t="s">
+      <c r="V38" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="T38" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="U38" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="V38" s="2" t="s">
-        <v>79</v>
-      </c>
       <c r="W38" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="39" spans="1:23" x14ac:dyDescent="0.15">
@@ -2944,67 +2944,67 @@
         <v>1</v>
       </c>
       <c r="B39" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="F39" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="C39" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="E39" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="F39" s="2" t="s">
+      <c r="G39" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="H39" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="I39" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="G39" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="H39" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="I39" s="2" t="s">
-        <v>79</v>
-      </c>
       <c r="J39" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="K39" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M39" s="2" t="s">
         <v>1</v>
       </c>
       <c r="N39" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="O39" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="P39" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="Q39" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="R39" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="S39" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="T39" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="U39" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="V39" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="W39" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="40" spans="1:23" x14ac:dyDescent="0.15">
@@ -3012,70 +3012,70 @@
         <v>2</v>
       </c>
       <c r="B40" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="F40" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="C40" s="2" t="s">
+      <c r="G40" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D40" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="E40" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="F40" s="2" t="s">
+      <c r="H40" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="I40" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="G40" s="2" t="s">
+      <c r="J40" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="H40" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="I40" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="J40" s="2" t="s">
-        <v>79</v>
-      </c>
       <c r="K40" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L40" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="M40" s="2" t="s">
         <v>2</v>
       </c>
       <c r="N40" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="O40" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="P40" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q40" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="R40" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="O40" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="P40" s="2" t="s">
+      <c r="S40" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="Q40" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="R40" s="2" t="s">
+      <c r="T40" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="U40" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="S40" s="2" t="s">
+      <c r="V40" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="T40" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="U40" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="V40" s="2" t="s">
-        <v>79</v>
-      </c>
       <c r="W40" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="41" spans="1:23" x14ac:dyDescent="0.15">
@@ -3083,67 +3083,67 @@
         <v>3</v>
       </c>
       <c r="B41" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="F41" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="C41" s="2" t="s">
+      <c r="G41" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D41" s="2" t="s">
+      <c r="H41" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="E41" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="F41" s="2" t="s">
+      <c r="I41" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="G41" s="2" t="s">
+      <c r="J41" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="H41" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="I41" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="J41" s="2" t="s">
-        <v>79</v>
-      </c>
       <c r="K41" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M41" s="2" t="s">
         <v>3</v>
       </c>
       <c r="N41" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="O41" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="P41" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q41" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="R41" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="O41" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="P41" s="2" t="s">
+      <c r="S41" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="Q41" s="2" t="s">
+      <c r="T41" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="R41" s="2" t="s">
+      <c r="U41" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="S41" s="2" t="s">
+      <c r="V41" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="T41" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="U41" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="V41" s="2" t="s">
-        <v>79</v>
-      </c>
       <c r="W41" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="42" spans="1:23" x14ac:dyDescent="0.15">
@@ -3151,70 +3151,70 @@
         <v>4</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I42" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J42" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="K42" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L42" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="M42" s="2" t="s">
         <v>4</v>
       </c>
       <c r="N42" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="O42" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="P42" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="Q42" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="R42" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="S42" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="T42" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="U42" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="V42" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="W42" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="43" spans="1:23" x14ac:dyDescent="0.15">
@@ -3222,70 +3222,70 @@
         <v>5</v>
       </c>
       <c r="B43" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C43" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="C43" s="2" t="s">
-        <v>81</v>
-      </c>
       <c r="D43" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I43" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J43" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="K43" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L43" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="M43" s="2" t="s">
         <v>5</v>
       </c>
       <c r="N43" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="O43" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="P43" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="Q43" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="R43" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="S43" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="T43" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="U43" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="V43" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="W43" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="44" spans="1:23" x14ac:dyDescent="0.15">
@@ -3293,67 +3293,67 @@
         <v>6</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C44" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D44" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="D44" s="2" t="s">
-        <v>85</v>
-      </c>
       <c r="E44" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I44" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J44" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="K44" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M44" s="2" t="s">
         <v>6</v>
       </c>
       <c r="N44" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="O44" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="P44" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="Q44" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="R44" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="S44" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="T44" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="U44" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="V44" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="W44" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="45" spans="1:23" x14ac:dyDescent="0.15">
@@ -3361,67 +3361,67 @@
         <v>7</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I45" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J45" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="K45" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="M45" s="2" t="s">
         <v>7</v>
       </c>
       <c r="N45" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="O45" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="P45" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="Q45" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="R45" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="S45" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="T45" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="U45" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="V45" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="W45" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="46" spans="1:23" x14ac:dyDescent="0.15">
@@ -3429,67 +3429,67 @@
         <v>8</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I46" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J46" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="K46" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M46" s="2" t="s">
         <v>8</v>
       </c>
       <c r="N46" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="O46" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="P46" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="Q46" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="R46" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="S46" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="T46" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="U46" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="V46" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="W46" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="47" spans="1:23" x14ac:dyDescent="0.15">
@@ -3497,94 +3497,94 @@
         <v>9</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G47" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I47" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J47" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K47" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="M47" s="2" t="s">
         <v>9</v>
       </c>
       <c r="N47" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="O47" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="P47" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q47" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="R47" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="S47" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="T47" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="U47" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="V47" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="W47" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="49" spans="1:12" ht="27" x14ac:dyDescent="0.15">
       <c r="A49" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B49" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C49" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D49" s="11"/>
+      <c r="E49" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F49" s="11"/>
+      <c r="G49" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C49" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="D49" s="14"/>
-      <c r="E49" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="F49" s="14"/>
-      <c r="G49" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="H49" s="12"/>
-      <c r="I49" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="J49" s="12"/>
+      <c r="H49" s="14"/>
+      <c r="I49" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="J49" s="14"/>
       <c r="K49" s="10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="L49" s="3"/>
     </row>
@@ -3593,26 +3593,26 @@
         <v>0</v>
       </c>
       <c r="B50" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="C50" s="14" t="s">
-        <v>98</v>
-      </c>
-      <c r="D50" s="14"/>
-      <c r="E50" s="14" t="s">
-        <v>99</v>
-      </c>
-      <c r="F50" s="14"/>
-      <c r="G50" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="H50" s="12"/>
-      <c r="I50" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="J50" s="12"/>
+        <v>89</v>
+      </c>
+      <c r="C50" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="D50" s="11"/>
+      <c r="E50" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="F50" s="11"/>
+      <c r="G50" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="H50" s="14"/>
+      <c r="I50" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="J50" s="14"/>
       <c r="K50" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L50" s="3"/>
     </row>
@@ -3621,26 +3621,26 @@
         <v>1</v>
       </c>
       <c r="B51" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="C51" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="C51" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="D51" s="11"/>
+      <c r="E51" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="D51" s="14"/>
-      <c r="E51" s="14" t="s">
-        <v>104</v>
-      </c>
-      <c r="F51" s="14"/>
-      <c r="G51" s="13" t="s">
-        <v>97</v>
-      </c>
-      <c r="H51" s="14"/>
-      <c r="I51" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="J51" s="12"/>
+      <c r="F51" s="11"/>
+      <c r="G51" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="H51" s="11"/>
+      <c r="I51" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="J51" s="14"/>
       <c r="K51" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L51" s="3"/>
     </row>
@@ -3649,26 +3649,26 @@
         <v>2</v>
       </c>
       <c r="B52" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="C52" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="D52" s="11"/>
+      <c r="E52" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="C52" s="14" t="s">
-        <v>101</v>
-      </c>
-      <c r="D52" s="14"/>
-      <c r="E52" s="14" t="s">
-        <v>96</v>
-      </c>
-      <c r="F52" s="14"/>
-      <c r="G52" s="11" t="s">
-        <v>109</v>
-      </c>
-      <c r="H52" s="12"/>
-      <c r="I52" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="J52" s="12"/>
+      <c r="F52" s="11"/>
+      <c r="G52" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="H52" s="14"/>
+      <c r="I52" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="J52" s="14"/>
       <c r="K52" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L52" s="3"/>
     </row>
@@ -3677,26 +3677,26 @@
         <v>3</v>
       </c>
       <c r="B53" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="C53" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="C53" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="D53" s="11"/>
+      <c r="E53" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="F53" s="11"/>
+      <c r="G53" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="D53" s="14"/>
-      <c r="E53" s="14" t="s">
-        <v>100</v>
-      </c>
-      <c r="F53" s="14"/>
-      <c r="G53" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="H53" s="12"/>
-      <c r="I53" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="J53" s="12"/>
+      <c r="H53" s="14"/>
+      <c r="I53" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="J53" s="14"/>
       <c r="K53" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L53" s="3"/>
     </row>
@@ -3705,29 +3705,29 @@
         <v>4</v>
       </c>
       <c r="B54" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="C54" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="C54" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="D54" s="11"/>
+      <c r="E54" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="F54" s="11"/>
+      <c r="G54" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="D54" s="14"/>
-      <c r="E54" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="F54" s="14"/>
-      <c r="G54" s="13" t="s">
-        <v>97</v>
-      </c>
-      <c r="H54" s="14"/>
-      <c r="I54" s="11" t="s">
-        <v>117</v>
-      </c>
-      <c r="J54" s="12"/>
+      <c r="H54" s="11"/>
+      <c r="I54" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="J54" s="14"/>
       <c r="K54" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L54" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.15">
@@ -3735,26 +3735,26 @@
         <v>5</v>
       </c>
       <c r="B55" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="C55" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="D55" s="14"/>
-      <c r="E55" s="14" t="s">
-        <v>107</v>
-      </c>
-      <c r="F55" s="14"/>
-      <c r="G55" s="11" t="s">
-        <v>110</v>
-      </c>
-      <c r="H55" s="12"/>
-      <c r="I55" s="11" t="s">
-        <v>118</v>
-      </c>
-      <c r="J55" s="12"/>
+        <v>92</v>
+      </c>
+      <c r="C55" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="D55" s="11"/>
+      <c r="E55" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="F55" s="11"/>
+      <c r="G55" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="H55" s="14"/>
+      <c r="I55" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="J55" s="14"/>
       <c r="K55" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L55" s="3"/>
     </row>
@@ -3763,26 +3763,26 @@
         <v>6</v>
       </c>
       <c r="B56" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="C56" s="14" t="s">
-        <v>100</v>
-      </c>
-      <c r="D56" s="14"/>
-      <c r="E56" s="14" t="s">
-        <v>100</v>
-      </c>
-      <c r="F56" s="14"/>
-      <c r="G56" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="H56" s="12"/>
-      <c r="I56" s="11" t="s">
-        <v>119</v>
-      </c>
-      <c r="J56" s="12"/>
+        <v>92</v>
+      </c>
+      <c r="C56" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="D56" s="11"/>
+      <c r="E56" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="F56" s="11"/>
+      <c r="G56" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="H56" s="14"/>
+      <c r="I56" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="J56" s="14"/>
       <c r="K56" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L56" s="3"/>
     </row>
@@ -3791,26 +3791,26 @@
         <v>7</v>
       </c>
       <c r="B57" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="C57" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="D57" s="14"/>
-      <c r="E57" s="14" t="s">
-        <v>108</v>
-      </c>
-      <c r="F57" s="14"/>
-      <c r="G57" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="H57" s="12"/>
-      <c r="I57" s="11" t="s">
-        <v>120</v>
-      </c>
-      <c r="J57" s="12"/>
+        <v>92</v>
+      </c>
+      <c r="C57" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="D57" s="11"/>
+      <c r="E57" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="F57" s="11"/>
+      <c r="G57" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="H57" s="14"/>
+      <c r="I57" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="J57" s="14"/>
       <c r="K57" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L57" s="3"/>
     </row>
@@ -3819,26 +3819,26 @@
         <v>8</v>
       </c>
       <c r="B58" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="C58" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="D58" s="14"/>
-      <c r="E58" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="F58" s="14"/>
-      <c r="G58" s="11" t="s">
-        <v>111</v>
-      </c>
-      <c r="H58" s="12"/>
-      <c r="I58" s="11" t="s">
-        <v>120</v>
-      </c>
-      <c r="J58" s="12"/>
+        <v>92</v>
+      </c>
+      <c r="C58" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="D58" s="11"/>
+      <c r="E58" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="F58" s="11"/>
+      <c r="G58" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="H58" s="14"/>
+      <c r="I58" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="J58" s="14"/>
       <c r="K58" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L58" s="3"/>
     </row>
@@ -3847,31 +3847,67 @@
         <v>9</v>
       </c>
       <c r="B59" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="C59" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="D59" s="14"/>
-      <c r="E59" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="F59" s="14"/>
-      <c r="G59" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="H59" s="12"/>
-      <c r="I59" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="J59" s="12"/>
+        <v>17</v>
+      </c>
+      <c r="C59" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="D59" s="11"/>
+      <c r="E59" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="F59" s="11"/>
+      <c r="G59" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="H59" s="14"/>
+      <c r="I59" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="J59" s="14"/>
       <c r="K59" s="10" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="L59" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="44">
+    <mergeCell ref="I54:J54"/>
+    <mergeCell ref="I49:J49"/>
+    <mergeCell ref="I50:J50"/>
+    <mergeCell ref="I51:J51"/>
+    <mergeCell ref="I52:J52"/>
+    <mergeCell ref="I53:J53"/>
+    <mergeCell ref="G49:H49"/>
+    <mergeCell ref="G50:H50"/>
+    <mergeCell ref="G51:H51"/>
+    <mergeCell ref="G52:H52"/>
+    <mergeCell ref="G53:H53"/>
+    <mergeCell ref="G57:H57"/>
+    <mergeCell ref="G58:H58"/>
+    <mergeCell ref="G59:H59"/>
+    <mergeCell ref="I55:J55"/>
+    <mergeCell ref="I56:J56"/>
+    <mergeCell ref="I57:J57"/>
+    <mergeCell ref="I58:J58"/>
+    <mergeCell ref="I59:J59"/>
+    <mergeCell ref="E54:F54"/>
+    <mergeCell ref="C54:D54"/>
+    <mergeCell ref="G54:H54"/>
+    <mergeCell ref="G55:H55"/>
+    <mergeCell ref="G56:H56"/>
+    <mergeCell ref="E55:F55"/>
+    <mergeCell ref="E56:F56"/>
+    <mergeCell ref="E49:F49"/>
+    <mergeCell ref="E50:F50"/>
+    <mergeCell ref="E51:F51"/>
+    <mergeCell ref="E52:F52"/>
+    <mergeCell ref="E53:F53"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="C51:D51"/>
+    <mergeCell ref="C52:D52"/>
+    <mergeCell ref="C53:D53"/>
     <mergeCell ref="E57:F57"/>
     <mergeCell ref="E58:F58"/>
     <mergeCell ref="E59:F59"/>
@@ -3880,42 +3916,6 @@
     <mergeCell ref="C57:D57"/>
     <mergeCell ref="C58:D58"/>
     <mergeCell ref="C59:D59"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="C50:D50"/>
-    <mergeCell ref="C51:D51"/>
-    <mergeCell ref="C52:D52"/>
-    <mergeCell ref="C53:D53"/>
-    <mergeCell ref="E49:F49"/>
-    <mergeCell ref="E50:F50"/>
-    <mergeCell ref="E51:F51"/>
-    <mergeCell ref="E52:F52"/>
-    <mergeCell ref="E53:F53"/>
-    <mergeCell ref="E54:F54"/>
-    <mergeCell ref="C54:D54"/>
-    <mergeCell ref="G54:H54"/>
-    <mergeCell ref="G55:H55"/>
-    <mergeCell ref="G56:H56"/>
-    <mergeCell ref="E55:F55"/>
-    <mergeCell ref="E56:F56"/>
-    <mergeCell ref="G57:H57"/>
-    <mergeCell ref="G58:H58"/>
-    <mergeCell ref="G59:H59"/>
-    <mergeCell ref="I55:J55"/>
-    <mergeCell ref="I56:J56"/>
-    <mergeCell ref="I57:J57"/>
-    <mergeCell ref="I58:J58"/>
-    <mergeCell ref="I59:J59"/>
-    <mergeCell ref="G49:H49"/>
-    <mergeCell ref="G50:H50"/>
-    <mergeCell ref="G51:H51"/>
-    <mergeCell ref="G52:H52"/>
-    <mergeCell ref="G53:H53"/>
-    <mergeCell ref="I54:J54"/>
-    <mergeCell ref="I49:J49"/>
-    <mergeCell ref="I50:J50"/>
-    <mergeCell ref="I51:J51"/>
-    <mergeCell ref="I52:J52"/>
-    <mergeCell ref="I53:J53"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>